<commit_message>
t5 - training stats, and t5 inference result updated
</commit_message>
<xml_diff>
--- a/Result and Analysis Section/Second pass model outputs/all_publication_inference_test.xlsx
+++ b/Result and Analysis Section/Second pass model outputs/all_publication_inference_test.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27029"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\parzi\OneDrive - Tribhuvan University\Desktop\Major Project\CODE\BCS Code\BCS-ALL-Code\Crossword Solver\Result and Analysis Section\Second pass model outputs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{790961DB-3163-41CF-90CF-0585AC63FE98}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{35B3EE85-0789-4E04-800B-44D1371C10A3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13020"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="all_publication_inference_test" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="13">
   <si>
     <t>Source</t>
   </si>
@@ -57,11 +57,14 @@
   <si>
     <t>S.N.</t>
   </si>
+  <si>
+    <t># Puzzles</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="19" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -628,14 +631,8 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -651,17 +648,26 @@
     <xf numFmtId="0" fontId="18" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="42">
@@ -1017,202 +1023,222 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H7"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:I7"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H14" sqref="H14"/>
+      <selection activeCell="I14" sqref="I14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="19.140625" customWidth="1"/>
-    <col min="3" max="3" width="14" customWidth="1"/>
-    <col min="4" max="4" width="13" customWidth="1"/>
-    <col min="5" max="5" width="14.7109375" customWidth="1"/>
-    <col min="6" max="6" width="13.7109375" customWidth="1"/>
-    <col min="7" max="7" width="12.85546875" customWidth="1"/>
-    <col min="8" max="8" width="14" customWidth="1"/>
+    <col min="3" max="3" width="14.5703125" customWidth="1"/>
+    <col min="4" max="4" width="14" customWidth="1"/>
+    <col min="5" max="5" width="13" customWidth="1"/>
+    <col min="6" max="6" width="14.7109375" customWidth="1"/>
+    <col min="7" max="7" width="13.7109375" customWidth="1"/>
+    <col min="8" max="8" width="12.85546875" customWidth="1"/>
+    <col min="9" max="9" width="14" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="D1" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="D1" s="2"/>
-      <c r="E1" s="2"/>
-      <c r="F1" s="2" t="s">
+      <c r="E1" s="8"/>
+      <c r="F1" s="8"/>
+      <c r="G1" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="G1" s="2"/>
-      <c r="H1" s="2"/>
+      <c r="H1" s="8"/>
+      <c r="I1" s="8"/>
     </row>
-    <row r="2" spans="1:8" ht="38.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="7"/>
-      <c r="B2" s="8"/>
-      <c r="C2" s="3" t="s">
+    <row r="2" spans="1:9" ht="38.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="11"/>
+      <c r="B2" s="9"/>
+      <c r="C2" s="12"/>
+      <c r="D2" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="D2" s="3" t="s">
+      <c r="E2" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="E2" s="3" t="s">
+      <c r="F2" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="F2" s="3" t="s">
+      <c r="G2" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="G2" s="3" t="s">
+      <c r="H2" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="H2" s="3" t="s">
+      <c r="I2" s="1" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="4">
+    <row r="3" spans="1:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="2">
         <v>1</v>
       </c>
-      <c r="B3" s="9" t="s">
+      <c r="B3" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="9">
+      <c r="C3" s="5">
+        <v>89</v>
+      </c>
+      <c r="D3" s="5">
         <v>99.49</v>
       </c>
-      <c r="D3" s="9">
+      <c r="E3" s="5">
         <v>97.8</v>
       </c>
-      <c r="E3" s="9">
+      <c r="F3" s="5">
         <v>76.400000000000006</v>
       </c>
-      <c r="F3" s="9">
+      <c r="G3" s="5">
         <v>99.86</v>
       </c>
-      <c r="G3" s="9">
+      <c r="H3" s="5">
         <v>99.34</v>
       </c>
-      <c r="H3" s="9">
+      <c r="I3" s="5">
         <v>91.01</v>
       </c>
     </row>
-    <row r="4" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="5">
+    <row r="4" spans="1:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="3">
         <v>2</v>
       </c>
-      <c r="B4" s="10" t="s">
+      <c r="B4" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="C4" s="10">
+      <c r="C4" s="6">
+        <v>100</v>
+      </c>
+      <c r="D4" s="6">
         <v>99.73</v>
       </c>
-      <c r="D4" s="10">
+      <c r="E4" s="6">
         <v>98.91</v>
       </c>
-      <c r="E4" s="10">
+      <c r="F4" s="6">
         <v>75</v>
       </c>
-      <c r="F4" s="10">
+      <c r="G4" s="6">
         <v>99.93</v>
       </c>
-      <c r="G4" s="10">
+      <c r="H4" s="6">
         <v>99.66</v>
       </c>
-      <c r="H4" s="10">
+      <c r="I4" s="6">
         <v>90</v>
       </c>
     </row>
-    <row r="5" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="5">
+    <row r="5" spans="1:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="3">
         <v>3</v>
       </c>
-      <c r="B5" s="10" t="s">
+      <c r="B5" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="C5" s="10">
+      <c r="C5" s="6">
+        <v>140</v>
+      </c>
+      <c r="D5" s="6">
         <v>99.81</v>
       </c>
-      <c r="D5" s="10">
+      <c r="E5" s="6">
         <v>99.23</v>
       </c>
-      <c r="E5" s="10">
+      <c r="F5" s="6">
         <v>80.709999999999994</v>
       </c>
-      <c r="F5" s="10">
+      <c r="G5" s="6">
         <v>99.99</v>
       </c>
-      <c r="G5" s="10">
+      <c r="H5" s="6">
         <v>99.93</v>
       </c>
-      <c r="H5" s="10">
+      <c r="I5" s="6">
         <v>97.14</v>
       </c>
     </row>
-    <row r="6" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="5">
+    <row r="6" spans="1:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="3">
         <v>4</v>
       </c>
-      <c r="B6" s="10" t="s">
+      <c r="B6" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="C6" s="10">
+      <c r="C6" s="6">
+        <v>79</v>
+      </c>
+      <c r="D6" s="6">
         <v>99.36</v>
       </c>
-      <c r="D6" s="10">
+      <c r="E6" s="6">
         <v>97.61</v>
       </c>
-      <c r="E6" s="10">
+      <c r="F6" s="6">
         <v>55.7</v>
       </c>
-      <c r="F6" s="10">
+      <c r="G6" s="6">
         <v>99.81</v>
       </c>
-      <c r="G6" s="10">
+      <c r="H6" s="6">
         <v>99.18</v>
       </c>
-      <c r="H6" s="10">
+      <c r="I6" s="6">
         <v>79.75</v>
       </c>
     </row>
-    <row r="7" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="6">
+    <row r="7" spans="1:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="4">
         <v>5</v>
       </c>
-      <c r="B7" s="11" t="s">
+      <c r="B7" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="C7" s="11">
+      <c r="C7" s="7">
+        <v>125</v>
+      </c>
+      <c r="D7" s="7">
         <v>99.38</v>
       </c>
-      <c r="D7" s="11">
+      <c r="E7" s="7">
         <v>97.65</v>
       </c>
-      <c r="E7" s="11">
+      <c r="F7" s="7">
         <v>56</v>
       </c>
-      <c r="F7" s="11">
+      <c r="G7" s="7">
         <v>99.76</v>
       </c>
-      <c r="G7" s="11">
+      <c r="H7" s="7">
         <v>99.18</v>
       </c>
-      <c r="H7" s="11">
+      <c r="I7" s="7">
         <v>83.2</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="4">
-    <mergeCell ref="C1:E1"/>
-    <mergeCell ref="F1:H1"/>
+  <mergeCells count="5">
+    <mergeCell ref="D1:F1"/>
+    <mergeCell ref="G1:I1"/>
     <mergeCell ref="B1:B2"/>
     <mergeCell ref="A1:A2"/>
+    <mergeCell ref="C1:C2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <legacyDrawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>